<commit_message>
Did my first gist import. Very slick.
</commit_message>
<xml_diff>
--- a/SuperXLOOKUP.xlsx
+++ b/SuperXLOOKUP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{93EEFA81-D8C6-409C-9771-491BCA8D6809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{3E23EBAA-1084-400B-BE20-550B3BE913FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -16,7 +16,10 @@
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_fSUPERXLOOKUP">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode,     IF(         COLUMNS(_xlpm.lookup_value) = 1,         IFERROR(             INDEX(                 _xlpm.return_array,                 _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode),                 _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))             ),             IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)         ),         IFERROR(             INDEX(                 _xlpm.return_array,                 _xlfn.SEQUENCE(ROWS(_xlpm.return_array)),                 _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)             ),             IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)         )     ) )</definedName>
+    <definedName name="_fIndex">_xlfn.LAMBDA(_xlpm.d,_xlpm.r, INDEX(_xlpm.d, _xlpm.r, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.d))))</definedName>
+    <definedName name="_fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat, _xlfn.LET(_xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , -1), _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , 1), _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , -1), _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , 1), IF(_xlpm.xmin = _xlpm.xmax, _xlpm.ymin, (_xlpm.ymin * (_xlpm.xmax - _xlpm.x) + _xlpm.ymax * (_xlpm.x - _xlpm.xmin)) / (_xlpm.xmax - _xlpm.xmin))))</definedName>
+    <definedName name="_fSUPER">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode,     IF(         COLUMNS(_xlpm.lookup_value) = 1,         IFERROR(             INDEX(                 _xlpm.return_array,                 _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode),                 _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))             ),             IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)         ),         IFERROR(             INDEX(                 _xlpm.return_array,                 _xlfn.SEQUENCE(ROWS(_xlpm.return_array)),                 _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)             ),             IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)         )     ) )</definedName>
+    <definedName name="_fSUPERXLOOKUP">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode, IF(COLUMNS(_xlpm.lookup_value) = 1, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode), _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)), IFERROR(INDEX(_xlpm.return_array, _xlfn.SEQUENCE(ROWS(_xlpm.return_array)), _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found))))</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -75,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Item</t>
   </si>
@@ -117,6 +120,15 @@
   </si>
   <si>
     <t>Indigo</t>
+  </si>
+  <si>
+    <t>Error Test</t>
+  </si>
+  <si>
+    <t>Lookup Test</t>
+  </si>
+  <si>
+    <t>Q5</t>
   </si>
 </sst>
 </file>
@@ -270,8 +282,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comment" xfId="8" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -916,7 +929,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="713" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -948,10 +961,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B9:L41"/>
+  <dimension ref="B9:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33:L37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -986,7 +999,15 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -1014,8 +1035,20 @@
       <c r="L33" t="s">
         <v>3</v>
       </c>
+      <c r="N33" t="s">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>12</v>
+      </c>
+      <c r="P33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1068,7 @@
         <v>6</v>
       </c>
       <c r="I34" cm="1">
-        <f t="array" ref="I34:L37">_fSUPERXLOOKUP(H34:H37,Table1[Item],Table1[[Q1]:[Q4]],0)</f>
+        <f t="array" ref="I34:L37">_fSUPER(H34:H37,Table1[Item],Table1[[Q1]:[Q4]],0)</f>
         <v>68</v>
       </c>
       <c r="J34">
@@ -1047,8 +1080,21 @@
       <c r="L34">
         <v>99</v>
       </c>
+      <c r="N34" t="s">
+        <v>4</v>
+      </c>
+      <c r="O34" cm="1">
+        <f t="array" ref="O34:Q41">_fSUPER(O33:Q33,Table1[[#Headers],[Q1]:[Q4]],Table1[[Q1]:[Q4]])</f>
+        <v>90</v>
+      </c>
+      <c r="P34">
+        <v>60</v>
+      </c>
+      <c r="Q34" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>5</v>
       </c>
@@ -1079,8 +1125,20 @@
       <c r="L35">
         <v>0</v>
       </c>
+      <c r="N35" t="s">
+        <v>5</v>
+      </c>
+      <c r="O35">
+        <v>79</v>
+      </c>
+      <c r="P35">
+        <v>85</v>
+      </c>
+      <c r="Q35" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>6</v>
       </c>
@@ -1111,8 +1169,20 @@
       <c r="L36">
         <v>85</v>
       </c>
+      <c r="N36" t="s">
+        <v>6</v>
+      </c>
+      <c r="O36">
+        <v>68</v>
+      </c>
+      <c r="P36">
+        <v>82</v>
+      </c>
+      <c r="Q36" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>7</v>
       </c>
@@ -1143,8 +1213,20 @@
       <c r="L37">
         <v>74</v>
       </c>
+      <c r="N37" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37">
+        <v>63</v>
+      </c>
+      <c r="P37">
+        <v>88</v>
+      </c>
+      <c r="Q37" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>8</v>
       </c>
@@ -1160,8 +1242,20 @@
       <c r="F38">
         <v>85</v>
       </c>
+      <c r="N38" t="s">
+        <v>8</v>
+      </c>
+      <c r="O38">
+        <v>54</v>
+      </c>
+      <c r="P38">
+        <v>53</v>
+      </c>
+      <c r="Q38" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>9</v>
       </c>
@@ -1177,8 +1271,20 @@
       <c r="F39">
         <v>74</v>
       </c>
+      <c r="N39" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39">
+        <v>67</v>
+      </c>
+      <c r="P39">
+        <v>84</v>
+      </c>
+      <c r="Q39" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>10</v>
       </c>
@@ -1194,8 +1300,20 @@
       <c r="F40">
         <v>96</v>
       </c>
+      <c r="N40" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40">
+        <v>69</v>
+      </c>
+      <c r="P40">
+        <v>98</v>
+      </c>
+      <c r="Q40" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>11</v>
       </c>
@@ -1210,19 +1328,32 @@
       </c>
       <c r="F41">
         <v>58</v>
+      </c>
+      <c r="N41" t="s">
+        <v>11</v>
+      </c>
+      <c r="O41">
+        <v>65</v>
+      </c>
+      <c r="P41">
+        <v>92</v>
+      </c>
+      <c r="Q41" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIABHAGUAbgBlAHIAYQB0AGUAIABhAG4AIABpAG4AZABlAHgAIABjAG8AbAB1AG0AbgAgAHQAaABlACAAaABlAGkAZwBoAHQAIABvAGYAIAB0AGgAZQAgAGQAYQB0AGEAIABkAFwAbgBfAGYASQBuAGQAZQB4AD0ATABBAE0AQgBEAEEAKABkACwAcgAsAEkATgBEAEUAWAAoAGQALAByACwAUwBFAFEAVQBFAE4AQwBFACgAMQAsAEMATwBMAFUATQBOAFMAKABkACkAKQApACkAOwBcAG4ALwAvACAAUwB1AHAAZQByAFgATABPAE8ASwBVAFAAXABuAF8AZgBTAFUAUABFAFIAWABMAE8ATwBLAFUAUAA9AEwAQQBNAEIARABBACgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALABsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAWwBpAGYAXwBuAG8AdABfAGYAbwB1AG4AZABdACwAWwBtAGEAdABjAGgAXwBtAG8AZABlAF0ALABbAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQBdACwAXABuACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABDAE8ATABVAE0ATgBTACgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUAKQAgAD0AIAAxACwAXABuACAAIAAgACAAIAAgACAAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAXwBhAHIAcgBhAHkALAAgAG0AYQB0AGMAaABfAG0AbwBkAGUALAAgAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAQwBPAEwAVQBNAE4AUwAoAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACkAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkALAAgAE4AQQAoACkALAAgAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABJAEYARQBSAFIATwBSACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkATgBEAEUAWAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBFAFEAVQBFAE4AQwBFACgAUgBPAFcAUwAoAHIAZQB0AHUAcgBuAF8AYQByAHIAYQB5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFgATQBBAFQAQwBIACgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALAAgAGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAIABtAGEAdABjAGgAXwBtAG8AZABlACwAIABzAGUAYQByAGMAaABfAG0AbwBkAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkALAAgAE4AQQAoACkALAAgAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8ALwAgAEwAaQBuAGUAYQByACAASQBuAHQAZQByAHAAbwBsAGEAdABpAG8AbgAgAEYAbwByAG0AdQBsAGEAXABuAF8AZgBJAG4AdABlAHIAcAA9AEwAQQBNAEIARABBACgAeAAsAHgAZABhAHQALAB5AGQAYQB0ACwAXABuACAAIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAIAB4AG0AaQBuACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB4AGQAYQB0ACwALAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAB4AG0AYQB4ACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB4AGQAYQB0ACwALAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAeQBtAGkAbgAsACAAWABMAE8ATwBLAFUAUAAoAHgALAB4AGQAYQB0ACwAeQBkAGEAdAAsACwALQAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAeQBtAGEAeAAsACAAWABMAE8ATwBLAFUAUAAoAHgALAB4AGQAYQB0ACwAeQBkAGEAdAAsACwAMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgAEkARgAoAHgAbQBpAG4APQB4AG0AYQB4ACwAeQBtAGkAbgAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAHkAbQBpAG4AKgAoAHgAbQBhAHgALQB4ACkAKwB5AG0AYQB4ACoAKAB4AC0AeABtAGkAbgApACkALwAoAHgAbQBhAHgALQB4AG0AaQBuACkAKQBcAG4AIAAgACAAIAAgACkAXABuACkAIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbACIAXwBmAEkAbgBkAGUAeAAiACwAIgBfAGYAUwBVAFAARQBSAFgATABPAE8ASwBVAFAAIgAsACIAXwBmAEkAbgB0AGUAcgBwACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIARABNAFkAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
I think this done.
</commit_message>
<xml_diff>
--- a/SuperXLOOKUP.xlsx
+++ b/SuperXLOOKUP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{3E23EBAA-1084-400B-BE20-550B3BE913FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{4660789D-F786-45CE-9BD4-099F23E08C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -42,9 +42,8 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -55,25 +54,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
@@ -583,13 +568,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>385440</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>95133</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -627,13 +612,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>565090</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>147080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -667,70 +652,176 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>36195</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58907755-C7ED-445D-BA50-7A801D3EC7B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2200275" cy="472440"/>
+          <a:chOff x="3162301" y="274265"/>
+          <a:chExt cx="2198370" cy="477072"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="TextBox 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF07FD3-FD2A-1D81-5EBA-4D37D55FA0D9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3162301" y="274265"/>
+            <a:ext cx="809778" cy="477072"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="91440" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1"/>
+              <a:t>FROM:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1"/>
+              <a:t>SUBJECT:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1"/>
+              <a:t>DATE:</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="TextBox 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFDC6503-5BB1-003C-94DE-7D09BDBCA761}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3908004" y="274265"/>
+            <a:ext cx="1452667" cy="459814"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="91440" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="0"/>
+              <a:t>Mark Biegert</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="0"/>
+              <a:t>SUPERXLOOKUP</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="0"/>
+              <a:t>21-Nov-2024</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>13</v>
-    <v>7</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_error">
-    <k n="errorType" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8EB621E-8042-49CC-9411-54C60EC6AA43}" name="Table1" displayName="Table1" ref="B33:F41" totalsRowShown="0">
-  <autoFilter ref="B33:F41" xr:uid="{D8EB621E-8042-49CC-9411-54C60EC6AA43}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8EB621E-8042-49CC-9411-54C60EC6AA43}" name="Table1" displayName="Table1" ref="B14:F22" totalsRowShown="0">
+  <autoFilter ref="B14:F22" xr:uid="{D8EB621E-8042-49CC-9411-54C60EC6AA43}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{65A5A0A7-0895-47C6-8597-3EA671B8BFAE}" name="Item"/>
     <tableColumn id="2" xr3:uid="{AEA0F09F-76B2-4E57-8EF8-38C9198045AE}" name="Q1"/>
@@ -961,10 +1052,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B9:Q41"/>
+  <dimension ref="B12:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -973,372 +1064,346 @@
     <col min="3" max="6" width="4.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E9" t="e" cm="1" vm="1">
-        <f t="array" ref="E9">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode,
-    IF(
-        COLUMNS(_xlpm.lookup_value) = 1,
-        IFERROR(
-            INDEX(
-                _xlpm.return_array,
-                _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode),
-                _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))
-            ),
-            IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)
-        ),
-        IFERROR(
-            INDEX(
-                _xlpm.return_array,
-                _xlfn.SEQUENCE(ROWS(_xlpm.return_array)),
-                _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)
-            ),
-            IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)
-        )
-    )
-)</f>
-        <v>#VALUE!</v>
+    <row r="12" spans="2:17" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="31" spans="8:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="H31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>14</v>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+      <c r="E15">
+        <v>77</v>
+      </c>
+      <c r="F15">
+        <v>54</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" cm="1">
+        <f t="array" ref="I15:L18">_fSUPER(H15:H18,Table1[Item],Table1[[Q1]:[Q4]],0)</f>
+        <v>68</v>
+      </c>
+      <c r="J15">
+        <v>82</v>
+      </c>
+      <c r="K15">
+        <v>66</v>
+      </c>
+      <c r="L15">
+        <v>99</v>
+      </c>
+      <c r="N15" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" cm="1">
+        <f t="array" ref="O15:Q22">_fSUPER(O14:Q14,Table1[[#Headers],[Q1]:[Q4]],Table1[[Q1]:[Q4]])</f>
+        <v>90</v>
+      </c>
+      <c r="P15">
+        <v>60</v>
+      </c>
+      <c r="Q15" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>79</v>
+      </c>
+      <c r="D16">
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <v>74</v>
+      </c>
+      <c r="F16">
+        <v>93</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33" t="s">
-        <v>3</v>
-      </c>
-      <c r="I33" t="s">
-        <v>12</v>
-      </c>
-      <c r="J33" t="s">
-        <v>1</v>
-      </c>
-      <c r="K33" t="s">
-        <v>2</v>
-      </c>
-      <c r="L33" t="s">
-        <v>3</v>
-      </c>
-      <c r="N33" t="s">
+      <c r="J16">
         <v>0</v>
       </c>
-      <c r="O33" t="s">
-        <v>12</v>
-      </c>
-      <c r="P33" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>16</v>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16">
+        <v>79</v>
+      </c>
+      <c r="P16">
+        <v>85</v>
+      </c>
+      <c r="Q16" t="e">
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>90</v>
-      </c>
-      <c r="D34">
-        <v>60</v>
-      </c>
-      <c r="E34">
-        <v>77</v>
-      </c>
-      <c r="F34">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>68</v>
+      </c>
+      <c r="D17">
+        <v>82</v>
+      </c>
+      <c r="E17">
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17">
         <v>54</v>
       </c>
-      <c r="H34" t="s">
+      <c r="J17">
+        <v>53</v>
+      </c>
+      <c r="K17">
+        <v>83</v>
+      </c>
+      <c r="L17">
+        <v>85</v>
+      </c>
+      <c r="N17" t="s">
         <v>6</v>
       </c>
-      <c r="I34" cm="1">
-        <f t="array" ref="I34:L37">_fSUPER(H34:H37,Table1[Item],Table1[[Q1]:[Q4]],0)</f>
+      <c r="O17">
         <v>68</v>
       </c>
-      <c r="J34">
+      <c r="P17">
         <v>82</v>
       </c>
-      <c r="K34">
-        <v>66</v>
-      </c>
-      <c r="L34">
-        <v>99</v>
-      </c>
-      <c r="N34" t="s">
-        <v>4</v>
-      </c>
-      <c r="O34" cm="1">
-        <f t="array" ref="O34:Q41">_fSUPER(O33:Q33,Table1[[#Headers],[Q1]:[Q4]],Table1[[Q1]:[Q4]])</f>
-        <v>90</v>
-      </c>
-      <c r="P34">
-        <v>60</v>
-      </c>
-      <c r="Q34" t="e">
+      <c r="Q17" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <v>79</v>
-      </c>
-      <c r="D35">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>63</v>
+      </c>
+      <c r="D18">
+        <v>88</v>
+      </c>
+      <c r="E18">
+        <v>61</v>
+      </c>
+      <c r="F18">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <v>67</v>
+      </c>
+      <c r="J18">
+        <v>84</v>
+      </c>
+      <c r="K18">
+        <v>82</v>
+      </c>
+      <c r="L18">
+        <v>74</v>
+      </c>
+      <c r="N18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18">
+        <v>63</v>
+      </c>
+      <c r="P18">
+        <v>88</v>
+      </c>
+      <c r="Q18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>54</v>
+      </c>
+      <c r="D19">
+        <v>53</v>
+      </c>
+      <c r="E19">
+        <v>83</v>
+      </c>
+      <c r="F19">
         <v>85</v>
       </c>
-      <c r="E35">
+      <c r="N19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O19">
+        <v>54</v>
+      </c>
+      <c r="P19">
+        <v>53</v>
+      </c>
+      <c r="Q19" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>67</v>
+      </c>
+      <c r="D20">
+        <v>84</v>
+      </c>
+      <c r="E20">
+        <v>82</v>
+      </c>
+      <c r="F20">
         <v>74</v>
       </c>
-      <c r="F35">
-        <v>93</v>
-      </c>
-      <c r="H35" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="N35" t="s">
-        <v>5</v>
-      </c>
-      <c r="O35">
-        <v>79</v>
-      </c>
-      <c r="P35">
-        <v>85</v>
-      </c>
-      <c r="Q35" t="e">
+      <c r="N20" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20">
+        <v>67</v>
+      </c>
+      <c r="P20">
+        <v>84</v>
+      </c>
+      <c r="Q20" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36">
-        <v>68</v>
-      </c>
-      <c r="D36">
-        <v>82</v>
-      </c>
-      <c r="E36">
-        <v>66</v>
-      </c>
-      <c r="F36">
-        <v>99</v>
-      </c>
-      <c r="H36" t="s">
-        <v>8</v>
-      </c>
-      <c r="I36">
-        <v>54</v>
-      </c>
-      <c r="J36">
-        <v>53</v>
-      </c>
-      <c r="K36">
-        <v>83</v>
-      </c>
-      <c r="L36">
-        <v>85</v>
-      </c>
-      <c r="N36" t="s">
-        <v>6</v>
-      </c>
-      <c r="O36">
-        <v>68</v>
-      </c>
-      <c r="P36">
-        <v>82</v>
-      </c>
-      <c r="Q36" t="e">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>69</v>
+      </c>
+      <c r="D21">
+        <v>98</v>
+      </c>
+      <c r="E21">
+        <v>52</v>
+      </c>
+      <c r="F21">
+        <v>96</v>
+      </c>
+      <c r="N21" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21">
+        <v>69</v>
+      </c>
+      <c r="P21">
+        <v>98</v>
+      </c>
+      <c r="Q21" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37">
-        <v>63</v>
-      </c>
-      <c r="D37">
-        <v>88</v>
-      </c>
-      <c r="E37">
-        <v>61</v>
-      </c>
-      <c r="F37">
-        <v>76</v>
-      </c>
-      <c r="H37" t="s">
-        <v>9</v>
-      </c>
-      <c r="I37">
-        <v>67</v>
-      </c>
-      <c r="J37">
-        <v>84</v>
-      </c>
-      <c r="K37">
-        <v>82</v>
-      </c>
-      <c r="L37">
-        <v>74</v>
-      </c>
-      <c r="N37" t="s">
-        <v>7</v>
-      </c>
-      <c r="O37">
-        <v>63</v>
-      </c>
-      <c r="P37">
-        <v>88</v>
-      </c>
-      <c r="Q37" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38">
-        <v>54</v>
-      </c>
-      <c r="D38">
-        <v>53</v>
-      </c>
-      <c r="E38">
-        <v>83</v>
-      </c>
-      <c r="F38">
-        <v>85</v>
-      </c>
-      <c r="N38" t="s">
-        <v>8</v>
-      </c>
-      <c r="O38">
-        <v>54</v>
-      </c>
-      <c r="P38">
-        <v>53</v>
-      </c>
-      <c r="Q38" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39">
-        <v>67</v>
-      </c>
-      <c r="D39">
-        <v>84</v>
-      </c>
-      <c r="E39">
-        <v>82</v>
-      </c>
-      <c r="F39">
-        <v>74</v>
-      </c>
-      <c r="N39" t="s">
-        <v>9</v>
-      </c>
-      <c r="O39">
-        <v>67</v>
-      </c>
-      <c r="P39">
-        <v>84</v>
-      </c>
-      <c r="Q39" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40">
-        <v>69</v>
-      </c>
-      <c r="D40">
-        <v>98</v>
-      </c>
-      <c r="E40">
-        <v>52</v>
-      </c>
-      <c r="F40">
-        <v>96</v>
-      </c>
-      <c r="N40" t="s">
-        <v>10</v>
-      </c>
-      <c r="O40">
-        <v>69</v>
-      </c>
-      <c r="P40">
-        <v>98</v>
-      </c>
-      <c r="Q40" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C41">
+      <c r="C22">
         <v>65</v>
       </c>
-      <c r="D41">
+      <c r="D22">
         <v>92</v>
       </c>
-      <c r="E41">
+      <c r="E22">
         <v>78</v>
       </c>
-      <c r="F41">
+      <c r="F22">
         <v>58</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N22" t="s">
         <v>11</v>
       </c>
-      <c r="O41">
+      <c r="O22">
         <v>65</v>
       </c>
-      <c r="P41">
+      <c r="P22">
         <v>92</v>
       </c>
-      <c r="Q41" t="e">
+      <c r="Q22" t="e">
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>